<commit_message>
Población con discapacidad en México
</commit_message>
<xml_diff>
--- a/Bases/Población con discapacidad por estados.xlsx
+++ b/Bases/Población con discapacidad por estados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvill\OneDrive\Escritorio\Trabajo_Aplicativo\07_Resultados\Tablas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github_Personal\Discapacidad_Mexico\Bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26420A1-1F0D-4C48-BAEF-324F2907712F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA54EF33-5B8F-4B6C-B790-01F8D352A591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34452" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Total</t>
   </si>
@@ -239,9 +239,6 @@
     <t>Zacatecas</t>
   </si>
   <si>
-    <t>FUENTE: INEGI. Censo de Población y Vivienda 2020. Cuestionario Básico.</t>
-  </si>
-  <si>
     <t>Población con discapacidad</t>
   </si>
   <si>
@@ -252,6 +249,12 @@
   </si>
   <si>
     <t>00</t>
+  </si>
+  <si>
+    <t>Población Total</t>
+  </si>
+  <si>
+    <t>Tasa de prevalencia</t>
   </si>
 </sst>
 </file>
@@ -318,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -342,6 +345,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -678,62 +684,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.06640625" style="3"/>
-    <col min="2" max="2" width="28.265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23" style="6" customWidth="1"/>
-    <col min="4" max="4" width="47" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.59765625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="40.3984375" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="3"/>
+    <col min="2" max="3" width="28.265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23" style="6" customWidth="1"/>
+    <col min="5" max="5" width="47" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="40.3984375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="15.06640625" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="6">
+        <v>126014024</v>
+      </c>
+      <c r="D2" s="6">
         <v>7168178</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E2" s="6">
         <v>264518</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="6">
         <v>6179890</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="6">
         <v>723770</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H2" s="9">
+        <v>5.6883970311113945</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -741,19 +762,25 @@
         <v>5</v>
       </c>
       <c r="C3" s="6">
+        <v>1425607</v>
+      </c>
+      <c r="D3" s="6">
         <v>83815</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="6">
         <v>3746</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="6">
         <v>71294</v>
       </c>
-      <c r="F3" s="6">
+      <c r="G3" s="6">
         <v>8775</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H3" s="9">
+        <v>5.8792500317408649</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -761,19 +788,25 @@
         <v>7</v>
       </c>
       <c r="C4" s="6">
+        <v>3769020</v>
+      </c>
+      <c r="D4" s="6">
         <v>188607</v>
       </c>
-      <c r="D4" s="6">
+      <c r="E4" s="6">
         <v>8517</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="6">
         <v>151945</v>
       </c>
-      <c r="F4" s="6">
+      <c r="G4" s="6">
         <v>28145</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H4" s="9">
+        <v>5.0041390069567155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -781,19 +814,25 @@
         <v>9</v>
       </c>
       <c r="C5" s="6">
+        <v>798447</v>
+      </c>
+      <c r="D5" s="6">
         <v>42117</v>
       </c>
-      <c r="D5" s="6">
+      <c r="E5" s="6">
         <v>1848</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
         <v>35383</v>
       </c>
-      <c r="F5" s="6">
+      <c r="G5" s="6">
         <v>4886</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H5" s="9">
+        <v>5.2748648313538657</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -801,19 +840,25 @@
         <v>11</v>
       </c>
       <c r="C6" s="6">
+        <v>928363</v>
+      </c>
+      <c r="D6" s="6">
         <v>59554</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="6">
         <v>2058</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="6">
         <v>52259</v>
       </c>
-      <c r="F6" s="6">
+      <c r="G6" s="6">
         <v>5237</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H6" s="9">
+        <v>6.4149476013154336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -821,19 +866,25 @@
         <v>13</v>
       </c>
       <c r="C7" s="6">
+        <v>3146771</v>
+      </c>
+      <c r="D7" s="6">
         <v>157685</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="6">
         <v>5358</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="6">
         <v>134816</v>
       </c>
-      <c r="F7" s="6">
+      <c r="G7" s="6">
         <v>17511</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H7" s="9">
+        <v>5.011009698513174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -841,19 +892,25 @@
         <v>15</v>
       </c>
       <c r="C8" s="6">
+        <v>731391</v>
+      </c>
+      <c r="D8" s="6">
         <v>45874</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="6">
         <v>1679</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F8" s="6">
         <v>39880</v>
       </c>
-      <c r="F8" s="6">
+      <c r="G8" s="6">
         <v>4315</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H8" s="9">
+        <v>6.2721581206222119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -861,19 +918,25 @@
         <v>17</v>
       </c>
       <c r="C9" s="6">
+        <v>5543828</v>
+      </c>
+      <c r="D9" s="6">
         <v>256758</v>
       </c>
-      <c r="D9" s="6">
+      <c r="E9" s="6">
         <v>6705</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <v>227878</v>
       </c>
-      <c r="F9" s="6">
+      <c r="G9" s="6">
         <v>22175</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H9" s="9">
+        <v>4.6314207439336137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -881,19 +944,25 @@
         <v>19</v>
       </c>
       <c r="C10" s="6">
+        <v>3741869</v>
+      </c>
+      <c r="D10" s="6">
         <v>200830</v>
       </c>
-      <c r="D10" s="6">
+      <c r="E10" s="6">
         <v>8433</v>
       </c>
-      <c r="E10" s="6">
+      <c r="F10" s="6">
         <v>167788</v>
       </c>
-      <c r="F10" s="6">
+      <c r="G10" s="6">
         <v>24609</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H10" s="9">
+        <v>5.3671039793215636</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -901,19 +970,25 @@
         <v>21</v>
       </c>
       <c r="C11" s="6">
+        <v>9209944</v>
+      </c>
+      <c r="D11" s="6">
         <v>589741</v>
       </c>
-      <c r="D11" s="6">
+      <c r="E11" s="6">
         <v>27132</v>
       </c>
-      <c r="E11" s="6">
+      <c r="F11" s="6">
         <v>493589</v>
       </c>
-      <c r="F11" s="6">
+      <c r="G11" s="6">
         <v>69020</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H11" s="9">
+        <v>6.4033071210856445</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -921,19 +996,25 @@
         <v>23</v>
       </c>
       <c r="C12" s="6">
+        <v>1832650</v>
+      </c>
+      <c r="D12" s="6">
         <v>115323</v>
       </c>
-      <c r="D12" s="6">
+      <c r="E12" s="6">
         <v>3903</v>
       </c>
-      <c r="E12" s="6">
+      <c r="F12" s="6">
         <v>101953</v>
       </c>
-      <c r="F12" s="6">
+      <c r="G12" s="6">
         <v>9467</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H12" s="9">
+        <v>6.2926909120672256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -941,19 +1022,25 @@
         <v>25</v>
       </c>
       <c r="C13" s="6">
+        <v>6166934</v>
+      </c>
+      <c r="D13" s="6">
         <v>333533</v>
       </c>
-      <c r="D13" s="6">
+      <c r="E13" s="6">
         <v>11609</v>
       </c>
-      <c r="E13" s="6">
+      <c r="F13" s="6">
         <v>285615</v>
       </c>
-      <c r="F13" s="6">
+      <c r="G13" s="6">
         <v>36309</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H13" s="9">
+        <v>5.4084087814139084</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -961,19 +1048,25 @@
         <v>27</v>
       </c>
       <c r="C14" s="6">
+        <v>3540685</v>
+      </c>
+      <c r="D14" s="6">
         <v>240098</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E14" s="6">
         <v>7641</v>
       </c>
-      <c r="E14" s="6">
+      <c r="F14" s="6">
         <v>213615</v>
       </c>
-      <c r="F14" s="6">
+      <c r="G14" s="6">
         <v>18842</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H14" s="9">
+        <v>6.781117213194622</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -981,19 +1074,25 @@
         <v>29</v>
       </c>
       <c r="C15" s="6">
+        <v>3082841</v>
+      </c>
+      <c r="D15" s="6">
         <v>189939</v>
       </c>
-      <c r="D15" s="6">
+      <c r="E15" s="6">
         <v>7023</v>
       </c>
-      <c r="E15" s="6">
+      <c r="F15" s="6">
         <v>166965</v>
       </c>
-      <c r="F15" s="6">
+      <c r="G15" s="6">
         <v>15951</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H15" s="9">
+        <v>6.1611675723788544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
@@ -1001,19 +1100,25 @@
         <v>31</v>
       </c>
       <c r="C16" s="6">
+        <v>8348151</v>
+      </c>
+      <c r="D16" s="6">
         <v>456844</v>
       </c>
-      <c r="D16" s="6">
+      <c r="E16" s="6">
         <v>18039</v>
       </c>
-      <c r="E16" s="6">
+      <c r="F16" s="6">
         <v>386577</v>
       </c>
-      <c r="F16" s="6">
+      <c r="G16" s="6">
         <v>52228</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H16" s="9">
+        <v>5.4723974206983081</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1021,19 +1126,25 @@
         <v>33</v>
       </c>
       <c r="C17" s="6">
+        <v>16992418</v>
+      </c>
+      <c r="D17" s="6">
         <v>892132</v>
       </c>
-      <c r="D17" s="6">
+      <c r="E17" s="6">
         <v>34303</v>
       </c>
-      <c r="E17" s="6">
+      <c r="F17" s="6">
         <v>756531</v>
       </c>
-      <c r="F17" s="6">
+      <c r="G17" s="6">
         <v>101298</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H17" s="9">
+        <v>5.2501768730030065</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1041,19 +1152,25 @@
         <v>35</v>
       </c>
       <c r="C18" s="6">
+        <v>4748846</v>
+      </c>
+      <c r="D18" s="6">
         <v>292223</v>
       </c>
-      <c r="D18" s="6">
+      <c r="E18" s="6">
         <v>9453</v>
       </c>
-      <c r="E18" s="6">
+      <c r="F18" s="6">
         <v>258107</v>
       </c>
-      <c r="F18" s="6">
+      <c r="G18" s="6">
         <v>24663</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H18" s="9">
+        <v>6.1535581486533788</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1061,19 +1178,25 @@
         <v>37</v>
       </c>
       <c r="C19" s="6">
+        <v>1971520</v>
+      </c>
+      <c r="D19" s="6">
         <v>123623</v>
       </c>
-      <c r="D19" s="6">
+      <c r="E19" s="6">
         <v>4252</v>
       </c>
-      <c r="E19" s="6">
+      <c r="F19" s="6">
         <v>109255</v>
       </c>
-      <c r="F19" s="6">
+      <c r="G19" s="6">
         <v>10116</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H19" s="9">
+        <v>6.2704410809933453</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
@@ -1081,19 +1204,25 @@
         <v>39</v>
       </c>
       <c r="C20" s="6">
+        <v>1235456</v>
+      </c>
+      <c r="D20" s="6">
         <v>78121</v>
       </c>
-      <c r="D20" s="6">
+      <c r="E20" s="6">
         <v>3049</v>
       </c>
-      <c r="E20" s="6">
+      <c r="F20" s="6">
         <v>68216</v>
       </c>
-      <c r="F20" s="6">
+      <c r="G20" s="6">
         <v>6856</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H20" s="9">
+        <v>6.3232523052217164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
@@ -1101,19 +1230,25 @@
         <v>41</v>
       </c>
       <c r="C21" s="6">
+        <v>5784442</v>
+      </c>
+      <c r="D21" s="6">
         <v>265892</v>
       </c>
-      <c r="D21" s="6">
+      <c r="E21" s="6">
         <v>11187</v>
       </c>
-      <c r="E21" s="6">
+      <c r="F21" s="6">
         <v>220206</v>
       </c>
-      <c r="F21" s="6">
+      <c r="G21" s="6">
         <v>34499</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H21" s="9">
+        <v>4.5966750120409197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -1121,19 +1256,25 @@
         <v>43</v>
       </c>
       <c r="C22" s="6">
+        <v>4132148</v>
+      </c>
+      <c r="D22" s="6">
         <v>298525</v>
       </c>
-      <c r="D22" s="6">
+      <c r="E22" s="6">
         <v>8374</v>
       </c>
-      <c r="E22" s="6">
+      <c r="F22" s="6">
         <v>273876</v>
       </c>
-      <c r="F22" s="6">
+      <c r="G22" s="6">
         <v>16275</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H22" s="9">
+        <v>7.2244508183153169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
@@ -1141,19 +1282,25 @@
         <v>45</v>
       </c>
       <c r="C23" s="6">
+        <v>6583278</v>
+      </c>
+      <c r="D23" s="6">
         <v>341490</v>
       </c>
-      <c r="D23" s="6">
+      <c r="E23" s="6">
         <v>10949</v>
       </c>
-      <c r="E23" s="6">
+      <c r="F23" s="6">
         <v>300150</v>
       </c>
-      <c r="F23" s="6">
+      <c r="G23" s="6">
         <v>30391</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H23" s="9">
+        <v>5.1872334724433626</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -1161,19 +1308,25 @@
         <v>47</v>
       </c>
       <c r="C24" s="6">
+        <v>2368467</v>
+      </c>
+      <c r="D24" s="6">
         <v>115215</v>
       </c>
-      <c r="D24" s="6">
+      <c r="E24" s="6">
         <v>4961</v>
       </c>
-      <c r="E24" s="6">
+      <c r="F24" s="6">
         <v>96160</v>
       </c>
-      <c r="F24" s="6">
+      <c r="G24" s="6">
         <v>14094</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H24" s="9">
+        <v>4.8645389612774848</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -1181,19 +1334,25 @@
         <v>49</v>
       </c>
       <c r="C25" s="6">
+        <v>1857985</v>
+      </c>
+      <c r="D25" s="6">
         <v>80602</v>
       </c>
-      <c r="D25" s="6">
+      <c r="E25" s="6">
         <v>2924</v>
       </c>
-      <c r="E25" s="6">
+      <c r="F25" s="6">
         <v>67005</v>
       </c>
-      <c r="F25" s="6">
+      <c r="G25" s="6">
         <v>10673</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H25" s="9">
+        <v>4.3381405124368602</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -1201,19 +1360,25 @@
         <v>51</v>
       </c>
       <c r="C26" s="6">
+        <v>2822255</v>
+      </c>
+      <c r="D26" s="6">
         <v>167855</v>
       </c>
-      <c r="D26" s="6">
+      <c r="E26" s="6">
         <v>6933</v>
       </c>
-      <c r="E26" s="6">
+      <c r="F26" s="6">
         <v>143861</v>
       </c>
-      <c r="F26" s="6">
+      <c r="G26" s="6">
         <v>17061</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H26" s="9">
+        <v>5.947549034371451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
@@ -1221,19 +1386,25 @@
         <v>53</v>
       </c>
       <c r="C27" s="6">
+        <v>3026943</v>
+      </c>
+      <c r="D27" s="6">
         <v>172818</v>
       </c>
-      <c r="D27" s="6">
+      <c r="E27" s="6">
         <v>6681</v>
       </c>
-      <c r="E27" s="6">
+      <c r="F27" s="6">
         <v>147958</v>
       </c>
-      <c r="F27" s="6">
+      <c r="G27" s="6">
         <v>18179</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H27" s="9">
+        <v>5.7093245561611168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
@@ -1241,19 +1412,25 @@
         <v>55</v>
       </c>
       <c r="C28" s="6">
+        <v>2944840</v>
+      </c>
+      <c r="D28" s="6">
         <v>170661</v>
       </c>
-      <c r="D28" s="6">
+      <c r="E28" s="6">
         <v>7034</v>
       </c>
-      <c r="E28" s="6">
+      <c r="F28" s="6">
         <v>145473</v>
       </c>
-      <c r="F28" s="6">
+      <c r="G28" s="6">
         <v>18154</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H28" s="9">
+        <v>5.7952554298365957</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
@@ -1261,19 +1438,25 @@
         <v>57</v>
       </c>
       <c r="C29" s="6">
+        <v>2402598</v>
+      </c>
+      <c r="D29" s="6">
         <v>161110</v>
       </c>
-      <c r="D29" s="6">
+      <c r="E29" s="6">
         <v>3966</v>
       </c>
-      <c r="E29" s="6">
+      <c r="F29" s="6">
         <v>144653</v>
       </c>
-      <c r="F29" s="6">
+      <c r="G29" s="6">
         <v>12491</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H29" s="9">
+        <v>6.7056577921067113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -1281,19 +1464,25 @@
         <v>59</v>
       </c>
       <c r="C30" s="6">
+        <v>3527735</v>
+      </c>
+      <c r="D30" s="6">
         <v>198955</v>
       </c>
-      <c r="D30" s="6">
+      <c r="E30" s="6">
         <v>7450</v>
       </c>
-      <c r="E30" s="6">
+      <c r="F30" s="6">
         <v>169649</v>
       </c>
-      <c r="F30" s="6">
+      <c r="G30" s="6">
         <v>21856</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H30" s="9">
+        <v>5.63973767870886</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>60</v>
       </c>
@@ -1301,19 +1490,25 @@
         <v>61</v>
       </c>
       <c r="C31" s="6">
+        <v>1342977</v>
+      </c>
+      <c r="D31" s="6">
         <v>62697</v>
       </c>
-      <c r="D31" s="6">
+      <c r="E31" s="6">
         <v>2183</v>
       </c>
-      <c r="E31" s="6">
+      <c r="F31" s="6">
         <v>54323</v>
       </c>
-      <c r="F31" s="6">
+      <c r="G31" s="6">
         <v>6191</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H31" s="9">
+        <v>4.6685088426681922</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
@@ -1321,19 +1516,25 @@
         <v>63</v>
       </c>
       <c r="C32" s="6">
+        <v>8062579</v>
+      </c>
+      <c r="D32" s="6">
         <v>529391</v>
       </c>
-      <c r="D32" s="6">
+      <c r="E32" s="6">
         <v>17554</v>
       </c>
-      <c r="E32" s="6">
+      <c r="F32" s="6">
         <v>468990</v>
       </c>
-      <c r="F32" s="6">
+      <c r="G32" s="6">
         <v>42847</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H32" s="9">
+        <v>6.5660255856097649</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
@@ -1341,19 +1542,25 @@
         <v>65</v>
       </c>
       <c r="C33" s="6">
+        <v>2320898</v>
+      </c>
+      <c r="D33" s="6">
         <v>149222</v>
       </c>
-      <c r="D33" s="6">
+      <c r="E33" s="6">
         <v>6379</v>
       </c>
-      <c r="E33" s="6">
+      <c r="F33" s="6">
         <v>129986</v>
       </c>
-      <c r="F33" s="6">
+      <c r="G33" s="6">
         <v>12857</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H33" s="9">
+        <v>6.4294941009902198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>66</v>
       </c>
@@ -1361,35 +1568,23 @@
         <v>67</v>
       </c>
       <c r="C34" s="6">
+        <v>1622138</v>
+      </c>
+      <c r="D34" s="6">
         <v>106928</v>
       </c>
-      <c r="D34" s="6">
+      <c r="E34" s="6">
         <v>3195</v>
       </c>
-      <c r="E34" s="6">
+      <c r="F34" s="6">
         <v>95934</v>
       </c>
-      <c r="F34" s="6">
+      <c r="G34" s="6">
         <v>7799</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B39" s="5"/>
+      <c r="H34" s="9">
+        <v>6.5917942863060981</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>